<commit_message>
more function headers and test cases
</commit_message>
<xml_diff>
--- a/Assignment 1 Test Plan.xlsx
+++ b/Assignment 1 Test Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-taroem\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project 1 Folder\sinkthefleet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1368" yWindow="0" windowWidth="21672" windowHeight="8808"/>
+    <workbookView xWindow="2736" yWindow="0" windowWidth="21672" windowHeight="8808"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Expected Output</t>
   </si>
@@ -105,6 +105,36 @@
   </si>
   <si>
     <t>Check that you can redo the grid if you do not like it.</t>
+  </si>
+  <si>
+    <t>setBoardSize()</t>
+  </si>
+  <si>
+    <t>reprompt for grid size</t>
+  </si>
+  <si>
+    <t>Check that setBoardSize will ignore incorrect input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter bad input - test case 'h', '3', 3 lines of junk, '#@ &amp;(' </t>
+  </si>
+  <si>
+    <t>getPlayerName()</t>
+  </si>
+  <si>
+    <t>enter long name over 100 characters with spaces</t>
+  </si>
+  <si>
+    <t>should store name and display exact input</t>
+  </si>
+  <si>
+    <t>stores full name and displays exact output</t>
+  </si>
+  <si>
+    <t>Check that you can't break anything in the getPlayerName function</t>
+  </si>
+  <si>
+    <t>"You have a ship occupying that spot"</t>
   </si>
 </sst>
 </file>
@@ -487,20 +517,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="57.21875" bestFit="1" customWidth="1"/>
@@ -587,10 +617,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
@@ -659,6 +689,256 @@
       <c r="I6" s="8" t="s">
         <v>26</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="4">
+        <v>42762</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="4">
+        <v>42762</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>